<commit_message>
add visual census and beach seines protocols
</commit_message>
<xml_diff>
--- a/visual-census/final_spreadsheets/diver_visual_survey_data_entry_spreadsheet_marinegeo.xlsx
+++ b/visual-census/final_spreadsheets/diver_visual_survey_data_entry_spreadsheet_marinegeo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>definition</t>
   </si>
@@ -398,13 +398,10 @@
     <t xml:space="preserve">taxon_id</t>
   </si>
   <si>
-    <t xml:space="preserve">The unique identifier for a single taxon. This column should include ALL uniquie taxon_id entries from the fish survey data sheet</t>
+    <t xml:space="preserve">The unique identifier for a single taxon. This column should include ALL unique taxon_id entries from the fish survey data sheet</t>
   </si>
   <si>
     <t xml:space="preserve">fish survey data, taxa list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A unique string (typically 3 digits) used to identify a single taxon. See the 'TaxaList' sheet for a list of TaxaCodes</t>
   </si>
   <si>
     <t xml:space="preserve">transect</t>
@@ -1907,43 +1904,27 @@
     </row>
     <row r="50">
       <c r="A50" s="10" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>75</v>
+        <v>13</v>
       </c>
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="11"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
+      <c r="A51" s="11"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1997,7 +1978,7 @@
         <v>90</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>107</v>
@@ -2090,7 +2071,7 @@
         <v>90</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>107</v>

</xml_diff>